<commit_message>
Re-formatted and reuploaded the Gantt chart
</commit_message>
<xml_diff>
--- a/CSC 225 - gantt chart.xlsx
+++ b/CSC 225 - gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f7049284458a4f2/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E6BCE01-7448-419C-B037-7DB235922D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{4E6BCE01-7448-419C-B037-7DB235922D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2DA467E-26C1-416C-81B3-73402FA8FA09}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Becca and Lauryn</t>
   </si>
   <si>
-    <t>How to Play page</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>Stats</t>
+  </si>
+  <si>
+    <t>How to play page</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -968,22 +968,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -995,26 +992,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1033,18 +1021,6 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1068,6 +1044,18 @@
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1562,8 +1550,8 @@
   </sheetPr>
   <dimension ref="A1:BL26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1589,28 +1577,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="94">
+      <c r="Q1" s="93">
         <v>45324</v>
       </c>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93"/>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B2" s="76" t="s">
@@ -1622,28 +1610,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="92">
+      <c r="Q2" s="91">
         <v>1</v>
       </c>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="93"/>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="93"/>
-      <c r="Z2" s="93"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="92"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
@@ -1659,102 +1647,102 @@
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="99">
+      <c r="I4" s="88">
         <f>I5</f>
         <v>45320</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86">
         <f>P5</f>
         <v>45327</v>
       </c>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86">
         <f>W5</f>
         <v>45334</v>
       </c>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="86">
         <f>AD5</f>
         <v>45341</v>
       </c>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="97"/>
-      <c r="AG4" s="97"/>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="97"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="97">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="86">
         <f>AK5</f>
         <v>45348</v>
       </c>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="97"/>
-      <c r="AN4" s="97"/>
-      <c r="AO4" s="97"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="97">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="86"/>
+      <c r="AR4" s="86">
         <f>AR5</f>
         <v>45355</v>
       </c>
-      <c r="AS4" s="97"/>
-      <c r="AT4" s="97"/>
-      <c r="AU4" s="97"/>
-      <c r="AV4" s="97"/>
-      <c r="AW4" s="97"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="97">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="86"/>
+      <c r="AY4" s="86">
         <f>AY5</f>
         <v>45362</v>
       </c>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="97"/>
-      <c r="BB4" s="97"/>
-      <c r="BC4" s="97"/>
-      <c r="BD4" s="97"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="97">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="86">
         <f>BF5</f>
         <v>45369</v>
       </c>
-      <c r="BG4" s="97"/>
-      <c r="BH4" s="97"/>
-      <c r="BI4" s="97"/>
-      <c r="BJ4" s="97"/>
-      <c r="BK4" s="97"/>
-      <c r="BL4" s="98"/>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="86"/>
-      <c r="B5" s="87" t="s">
+      <c r="A5" s="96"/>
+      <c r="B5" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="89" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -1983,8 +1971,8 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="86"/>
-      <c r="B6" s="88"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="90"/>
       <c r="D6" s="90"/>
       <c r="E6" s="90"/>
@@ -2544,7 +2532,7 @@
         <v>45324</v>
       </c>
       <c r="F12" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5" t="e">
@@ -2623,7 +2611,7 @@
         <v>45365</v>
       </c>
       <c r="F13" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="5" t="e">
@@ -2702,7 +2690,7 @@
         <v>45365</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="5" t="e">
@@ -2781,7 +2769,7 @@
         <v>45365</v>
       </c>
       <c r="F15" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="5" t="e">
@@ -2860,7 +2848,7 @@
         <v>45365</v>
       </c>
       <c r="F16" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="5" t="e">
@@ -2926,385 +2914,385 @@
     </row>
     <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="13"/>
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="102">
+      <c r="D17" s="64">
         <v>0.1</v>
       </c>
-      <c r="E17" s="103">
+      <c r="E17" s="65">
         <v>45365</v>
       </c>
-      <c r="F17" s="103" t="s">
-        <v>47</v>
+      <c r="F17" s="65" t="s">
+        <v>46</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="45"/>
-      <c r="AA17" s="45"/>
-      <c r="AB17" s="45"/>
-      <c r="AC17" s="45"/>
-      <c r="AD17" s="45"/>
-      <c r="AE17" s="45"/>
-      <c r="AF17" s="45"/>
-      <c r="AG17" s="45"/>
-      <c r="AH17" s="45"/>
-      <c r="AI17" s="45"/>
-      <c r="AJ17" s="45"/>
-      <c r="AK17" s="45"/>
-      <c r="AL17" s="45"/>
-      <c r="AM17" s="45"/>
-      <c r="AN17" s="45"/>
-      <c r="AO17" s="45"/>
-      <c r="AP17" s="45"/>
-      <c r="AQ17" s="45"/>
-      <c r="AR17" s="45"/>
-      <c r="AS17" s="45"/>
-      <c r="AT17" s="45"/>
-      <c r="AU17" s="45"/>
-      <c r="AV17" s="45"/>
-      <c r="AW17" s="45"/>
-      <c r="AX17" s="45"/>
-      <c r="AY17" s="45"/>
-      <c r="AZ17" s="45"/>
-      <c r="BA17" s="45"/>
-      <c r="BB17" s="45"/>
-      <c r="BC17" s="45"/>
-      <c r="BD17" s="45"/>
-      <c r="BE17" s="45"/>
-      <c r="BF17" s="45"/>
-      <c r="BG17" s="45"/>
-      <c r="BH17" s="45"/>
-      <c r="BI17" s="45"/>
-      <c r="BJ17" s="45"/>
-      <c r="BK17" s="45"/>
-      <c r="BL17" s="45"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="51"/>
+      <c r="AG17" s="51"/>
+      <c r="AH17" s="51"/>
+      <c r="AI17" s="51"/>
+      <c r="AJ17" s="51"/>
+      <c r="AK17" s="51"/>
+      <c r="AL17" s="51"/>
+      <c r="AM17" s="51"/>
+      <c r="AN17" s="51"/>
+      <c r="AO17" s="51"/>
+      <c r="AP17" s="51"/>
+      <c r="AQ17" s="51"/>
+      <c r="AR17" s="51"/>
+      <c r="AS17" s="51"/>
+      <c r="AT17" s="51"/>
+      <c r="AU17" s="51"/>
+      <c r="AV17" s="51"/>
+      <c r="AW17" s="51"/>
+      <c r="AX17" s="51"/>
+      <c r="AY17" s="51"/>
+      <c r="AZ17" s="51"/>
+      <c r="BA17" s="51"/>
+      <c r="BB17" s="51"/>
+      <c r="BC17" s="51"/>
+      <c r="BD17" s="51"/>
+      <c r="BE17" s="51"/>
+      <c r="BF17" s="51"/>
+      <c r="BG17" s="51"/>
+      <c r="BH17" s="51"/>
+      <c r="BI17" s="51"/>
+      <c r="BJ17" s="51"/>
+      <c r="BK17" s="51"/>
+      <c r="BL17" s="51"/>
     </row>
     <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="13"/>
-      <c r="B18" s="100" t="s">
+      <c r="B18" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="102">
+      <c r="D18" s="64">
         <v>0.05</v>
       </c>
-      <c r="E18" s="103">
+      <c r="E18" s="65">
         <v>45365</v>
       </c>
-      <c r="F18" s="103" t="s">
-        <v>47</v>
+      <c r="F18" s="65" t="s">
+        <v>46</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="45"/>
-      <c r="W18" s="45"/>
-      <c r="X18" s="45"/>
-      <c r="Y18" s="45"/>
-      <c r="Z18" s="45"/>
-      <c r="AA18" s="45"/>
-      <c r="AB18" s="45"/>
-      <c r="AC18" s="45"/>
-      <c r="AD18" s="45"/>
-      <c r="AE18" s="45"/>
-      <c r="AF18" s="45"/>
-      <c r="AG18" s="45"/>
-      <c r="AH18" s="45"/>
-      <c r="AI18" s="45"/>
-      <c r="AJ18" s="45"/>
-      <c r="AK18" s="45"/>
-      <c r="AL18" s="45"/>
-      <c r="AM18" s="45"/>
-      <c r="AN18" s="45"/>
-      <c r="AO18" s="45"/>
-      <c r="AP18" s="45"/>
-      <c r="AQ18" s="45"/>
-      <c r="AR18" s="45"/>
-      <c r="AS18" s="45"/>
-      <c r="AT18" s="45"/>
-      <c r="AU18" s="45"/>
-      <c r="AV18" s="45"/>
-      <c r="AW18" s="45"/>
-      <c r="AX18" s="45"/>
-      <c r="AY18" s="45"/>
-      <c r="AZ18" s="45"/>
-      <c r="BA18" s="45"/>
-      <c r="BB18" s="45"/>
-      <c r="BC18" s="45"/>
-      <c r="BD18" s="45"/>
-      <c r="BE18" s="45"/>
-      <c r="BF18" s="45"/>
-      <c r="BG18" s="45"/>
-      <c r="BH18" s="45"/>
-      <c r="BI18" s="45"/>
-      <c r="BJ18" s="45"/>
-      <c r="BK18" s="45"/>
-      <c r="BL18" s="45"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+      <c r="AB18" s="51"/>
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="51"/>
+      <c r="AF18" s="51"/>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="51"/>
+      <c r="AI18" s="51"/>
+      <c r="AJ18" s="51"/>
+      <c r="AK18" s="51"/>
+      <c r="AL18" s="51"/>
+      <c r="AM18" s="51"/>
+      <c r="AN18" s="51"/>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="51"/>
+      <c r="AQ18" s="51"/>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="51"/>
+      <c r="AT18" s="51"/>
+      <c r="AU18" s="51"/>
+      <c r="AV18" s="51"/>
+      <c r="AW18" s="51"/>
+      <c r="AX18" s="51"/>
+      <c r="AY18" s="51"/>
+      <c r="AZ18" s="51"/>
+      <c r="BA18" s="51"/>
+      <c r="BB18" s="51"/>
+      <c r="BC18" s="51"/>
+      <c r="BD18" s="51"/>
+      <c r="BE18" s="51"/>
+      <c r="BF18" s="51"/>
+      <c r="BG18" s="51"/>
+      <c r="BH18" s="51"/>
+      <c r="BI18" s="51"/>
+      <c r="BJ18" s="51"/>
+      <c r="BK18" s="51"/>
+      <c r="BL18" s="51"/>
     </row>
     <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13"/>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="64">
+        <v>0</v>
+      </c>
+      <c r="E19" s="65">
+        <v>45365</v>
+      </c>
+      <c r="F19" s="65" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="101" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="102">
-        <v>0.05</v>
-      </c>
-      <c r="E19" s="103">
-        <v>45365</v>
-      </c>
-      <c r="F19" s="103" t="s">
-        <v>47</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="45"/>
-      <c r="W19" s="45"/>
-      <c r="X19" s="45"/>
-      <c r="Y19" s="45"/>
-      <c r="Z19" s="45"/>
-      <c r="AA19" s="45"/>
-      <c r="AB19" s="45"/>
-      <c r="AC19" s="45"/>
-      <c r="AD19" s="45"/>
-      <c r="AE19" s="45"/>
-      <c r="AF19" s="45"/>
-      <c r="AG19" s="45"/>
-      <c r="AH19" s="45"/>
-      <c r="AI19" s="45"/>
-      <c r="AJ19" s="45"/>
-      <c r="AK19" s="45"/>
-      <c r="AL19" s="45"/>
-      <c r="AM19" s="45"/>
-      <c r="AN19" s="45"/>
-      <c r="AO19" s="45"/>
-      <c r="AP19" s="45"/>
-      <c r="AQ19" s="45"/>
-      <c r="AR19" s="45"/>
-      <c r="AS19" s="45"/>
-      <c r="AT19" s="45"/>
-      <c r="AU19" s="45"/>
-      <c r="AV19" s="45"/>
-      <c r="AW19" s="45"/>
-      <c r="AX19" s="45"/>
-      <c r="AY19" s="45"/>
-      <c r="AZ19" s="45"/>
-      <c r="BA19" s="45"/>
-      <c r="BB19" s="45"/>
-      <c r="BC19" s="45"/>
-      <c r="BD19" s="45"/>
-      <c r="BE19" s="45"/>
-      <c r="BF19" s="45"/>
-      <c r="BG19" s="45"/>
-      <c r="BH19" s="45"/>
-      <c r="BI19" s="45"/>
-      <c r="BJ19" s="45"/>
-      <c r="BK19" s="45"/>
-      <c r="BL19" s="45"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="51"/>
+      <c r="AI19" s="51"/>
+      <c r="AJ19" s="51"/>
+      <c r="AK19" s="51"/>
+      <c r="AL19" s="51"/>
+      <c r="AM19" s="51"/>
+      <c r="AN19" s="51"/>
+      <c r="AO19" s="51"/>
+      <c r="AP19" s="51"/>
+      <c r="AQ19" s="51"/>
+      <c r="AR19" s="51"/>
+      <c r="AS19" s="51"/>
+      <c r="AT19" s="51"/>
+      <c r="AU19" s="51"/>
+      <c r="AV19" s="51"/>
+      <c r="AW19" s="51"/>
+      <c r="AX19" s="51"/>
+      <c r="AY19" s="51"/>
+      <c r="AZ19" s="51"/>
+      <c r="BA19" s="51"/>
+      <c r="BB19" s="51"/>
+      <c r="BC19" s="51"/>
+      <c r="BD19" s="51"/>
+      <c r="BE19" s="51"/>
+      <c r="BF19" s="51"/>
+      <c r="BG19" s="51"/>
+      <c r="BH19" s="51"/>
+      <c r="BI19" s="51"/>
+      <c r="BJ19" s="51"/>
+      <c r="BK19" s="51"/>
+      <c r="BL19" s="51"/>
     </row>
     <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="102">
+      <c r="D20" s="64">
         <v>0</v>
       </c>
-      <c r="E20" s="103" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="103" t="s">
-        <v>47</v>
+      <c r="E20" s="65">
+        <v>45365</v>
+      </c>
+      <c r="F20" s="65" t="s">
+        <v>46</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="45"/>
-      <c r="W20" s="45"/>
-      <c r="X20" s="45"/>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="45"/>
-      <c r="AB20" s="45"/>
-      <c r="AC20" s="45"/>
-      <c r="AD20" s="45"/>
-      <c r="AE20" s="45"/>
-      <c r="AF20" s="45"/>
-      <c r="AG20" s="45"/>
-      <c r="AH20" s="45"/>
-      <c r="AI20" s="45"/>
-      <c r="AJ20" s="45"/>
-      <c r="AK20" s="45"/>
-      <c r="AL20" s="45"/>
-      <c r="AM20" s="45"/>
-      <c r="AN20" s="45"/>
-      <c r="AO20" s="45"/>
-      <c r="AP20" s="45"/>
-      <c r="AQ20" s="45"/>
-      <c r="AR20" s="45"/>
-      <c r="AS20" s="45"/>
-      <c r="AT20" s="45"/>
-      <c r="AU20" s="45"/>
-      <c r="AV20" s="45"/>
-      <c r="AW20" s="45"/>
-      <c r="AX20" s="45"/>
-      <c r="AY20" s="45"/>
-      <c r="AZ20" s="45"/>
-      <c r="BA20" s="45"/>
-      <c r="BB20" s="45"/>
-      <c r="BC20" s="45"/>
-      <c r="BD20" s="45"/>
-      <c r="BE20" s="45"/>
-      <c r="BF20" s="45"/>
-      <c r="BG20" s="45"/>
-      <c r="BH20" s="45"/>
-      <c r="BI20" s="45"/>
-      <c r="BJ20" s="45"/>
-      <c r="BK20" s="45"/>
-      <c r="BL20" s="45"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="51"/>
+      <c r="AI20" s="51"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="51"/>
+      <c r="AL20" s="51"/>
+      <c r="AM20" s="51"/>
+      <c r="AN20" s="51"/>
+      <c r="AO20" s="51"/>
+      <c r="AP20" s="51"/>
+      <c r="AQ20" s="51"/>
+      <c r="AR20" s="51"/>
+      <c r="AS20" s="51"/>
+      <c r="AT20" s="51"/>
+      <c r="AU20" s="51"/>
+      <c r="AV20" s="51"/>
+      <c r="AW20" s="51"/>
+      <c r="AX20" s="51"/>
+      <c r="AY20" s="51"/>
+      <c r="AZ20" s="51"/>
+      <c r="BA20" s="51"/>
+      <c r="BB20" s="51"/>
+      <c r="BC20" s="51"/>
+      <c r="BD20" s="51"/>
+      <c r="BE20" s="51"/>
+      <c r="BF20" s="51"/>
+      <c r="BG20" s="51"/>
+      <c r="BH20" s="51"/>
+      <c r="BI20" s="51"/>
+      <c r="BJ20" s="51"/>
+      <c r="BK20" s="51"/>
+      <c r="BL20" s="51"/>
     </row>
     <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="13"/>
-      <c r="B21" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="101" t="s">
+      <c r="B21" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="102">
+      <c r="D21" s="64">
         <v>0</v>
       </c>
-      <c r="E21" s="103" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="103" t="s">
-        <v>47</v>
+      <c r="E21" s="65">
+        <v>45365</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>46</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="45"/>
-      <c r="V21" s="45"/>
-      <c r="W21" s="45"/>
-      <c r="X21" s="45"/>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="45"/>
-      <c r="AA21" s="45"/>
-      <c r="AB21" s="45"/>
-      <c r="AC21" s="45"/>
-      <c r="AD21" s="45"/>
-      <c r="AE21" s="45"/>
-      <c r="AF21" s="45"/>
-      <c r="AG21" s="45"/>
-      <c r="AH21" s="45"/>
-      <c r="AI21" s="45"/>
-      <c r="AJ21" s="45"/>
-      <c r="AK21" s="45"/>
-      <c r="AL21" s="45"/>
-      <c r="AM21" s="45"/>
-      <c r="AN21" s="45"/>
-      <c r="AO21" s="45"/>
-      <c r="AP21" s="45"/>
-      <c r="AQ21" s="45"/>
-      <c r="AR21" s="45"/>
-      <c r="AS21" s="45"/>
-      <c r="AT21" s="45"/>
-      <c r="AU21" s="45"/>
-      <c r="AV21" s="45"/>
-      <c r="AW21" s="45"/>
-      <c r="AX21" s="45"/>
-      <c r="AY21" s="45"/>
-      <c r="AZ21" s="45"/>
-      <c r="BA21" s="45"/>
-      <c r="BB21" s="45"/>
-      <c r="BC21" s="45"/>
-      <c r="BD21" s="45"/>
-      <c r="BE21" s="45"/>
-      <c r="BF21" s="45"/>
-      <c r="BG21" s="45"/>
-      <c r="BH21" s="45"/>
-      <c r="BI21" s="45"/>
-      <c r="BJ21" s="45"/>
-      <c r="BK21" s="45"/>
-      <c r="BL21" s="45"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="51"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="51"/>
+      <c r="AF21" s="51"/>
+      <c r="AG21" s="51"/>
+      <c r="AH21" s="51"/>
+      <c r="AI21" s="51"/>
+      <c r="AJ21" s="51"/>
+      <c r="AK21" s="51"/>
+      <c r="AL21" s="51"/>
+      <c r="AM21" s="51"/>
+      <c r="AN21" s="51"/>
+      <c r="AO21" s="51"/>
+      <c r="AP21" s="51"/>
+      <c r="AQ21" s="51"/>
+      <c r="AR21" s="51"/>
+      <c r="AS21" s="51"/>
+      <c r="AT21" s="51"/>
+      <c r="AU21" s="51"/>
+      <c r="AV21" s="51"/>
+      <c r="AW21" s="51"/>
+      <c r="AX21" s="51"/>
+      <c r="AY21" s="51"/>
+      <c r="AZ21" s="51"/>
+      <c r="BA21" s="51"/>
+      <c r="BB21" s="51"/>
+      <c r="BC21" s="51"/>
+      <c r="BD21" s="51"/>
+      <c r="BE21" s="51"/>
+      <c r="BF21" s="51"/>
+      <c r="BG21" s="51"/>
+      <c r="BH21" s="51"/>
+      <c r="BI21" s="51"/>
+      <c r="BJ21" s="51"/>
+      <c r="BK21" s="51"/>
+      <c r="BL21" s="51"/>
     </row>
     <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="13"/>
@@ -3458,6 +3446,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -3466,16 +3464,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D23">
     <cfRule type="dataBar" priority="23">
@@ -3491,6 +3479,11 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I4:BL21">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I9:BL10">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
@@ -3500,16 +3493,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:BL21">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL21">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
@@ -3686,12 +3674,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4007,29 +4006,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4056,20 +4055,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>